<commit_message>
add SCHISM station descr and name
</commit_message>
<xml_diff>
--- a/data/Stations_Importance.xlsx
+++ b/data/Stations_Importance.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\delta_salinity\scripts\DSP_code\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A69CF44-7AB7-4961-B6D7-54448C9C51A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46B99664-A13E-4C88-B1D7-E28FFE933137}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17790" xr2:uid="{DB7A9B06-FD48-4539-AA38-6D28440ECAB7}"/>
+    <workbookView xWindow="-28800" yWindow="0" windowWidth="14400" windowHeight="17550" xr2:uid="{DB7A9B06-FD48-4539-AA38-6D28440ECAB7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="147">
   <si>
     <t>Y</t>
   </si>
@@ -279,13 +279,211 @@
   </si>
   <si>
     <t>MRU</t>
+  </si>
+  <si>
+    <t>SCHISM</t>
+  </si>
+  <si>
+    <t>trp</t>
+  </si>
+  <si>
+    <t>DSM2 Description</t>
+  </si>
+  <si>
+    <t>CBP Intake at Tracy Pumping Plant</t>
+  </si>
+  <si>
+    <t>wci</t>
+  </si>
+  <si>
+    <t>West Canal near Clifton Court Intake</t>
+  </si>
+  <si>
+    <t>vcu</t>
+  </si>
+  <si>
+    <t>Victoria Canal</t>
+  </si>
+  <si>
+    <t>uni</t>
+  </si>
+  <si>
+    <t>Old River neart Middle River</t>
+  </si>
+  <si>
+    <t>obi</t>
+  </si>
+  <si>
+    <t>Old R at Bacon Island</t>
+  </si>
+  <si>
+    <t xml:space="preserve">old </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Old River at Tracy Blvd </t>
+  </si>
+  <si>
+    <t>Sacramento River at Port Chicago</t>
+  </si>
+  <si>
+    <t>pct</t>
+  </si>
+  <si>
+    <t>mal</t>
+  </si>
+  <si>
+    <t>Sacramento River at Collinsville</t>
+  </si>
+  <si>
+    <t>Sacramento River at Mallard Island</t>
+  </si>
+  <si>
+    <t>cse</t>
+  </si>
+  <si>
+    <t>emm2</t>
+  </si>
+  <si>
+    <t>Sacramento River at Emmaton</t>
+  </si>
+  <si>
+    <t>anh</t>
+  </si>
+  <si>
+    <t>San Joaquin at Antioch</t>
+  </si>
+  <si>
+    <t>jer</t>
+  </si>
+  <si>
+    <t>Jersey Point</t>
+  </si>
+  <si>
+    <t>bdl</t>
+  </si>
+  <si>
+    <t>Montezuma Slough near Beldons Landing</t>
+  </si>
+  <si>
+    <t>Rough and Ready Island</t>
+  </si>
+  <si>
+    <t>rri2</t>
+  </si>
+  <si>
+    <t>San Joaquin River at Brandt Bridge</t>
+  </si>
+  <si>
+    <t>bdt</t>
+  </si>
+  <si>
+    <t>Chadbourne Slough at Sunrise Duck Club</t>
+  </si>
+  <si>
+    <t>snc</t>
+  </si>
+  <si>
+    <t>Little Potato Slough at Terminous</t>
+  </si>
+  <si>
+    <t>lps</t>
+  </si>
+  <si>
+    <t>Dutch Sl below Jersey Island</t>
+  </si>
+  <si>
+    <t>dsj</t>
+  </si>
+  <si>
+    <t>Montezuma Slough at National Steel</t>
+  </si>
+  <si>
+    <t>nsl2</t>
+  </si>
+  <si>
+    <t>vol</t>
+  </si>
+  <si>
+    <t>Suisun Slough 300' south of Volanti Slough</t>
+  </si>
+  <si>
+    <t>tss</t>
+  </si>
+  <si>
+    <t>sss</t>
+  </si>
+  <si>
+    <t>Threemile Slough near San Joaquin River</t>
+  </si>
+  <si>
+    <t>Steamboat Slough btw Sacramento R and Sutter Sl</t>
+  </si>
+  <si>
+    <t>carqb</t>
+  </si>
+  <si>
+    <t>Carquinez Strait at Carquinez Bridge near Crockett</t>
+  </si>
+  <si>
+    <t>inb</t>
+  </si>
+  <si>
+    <t>CWD Rock Slough PP</t>
+  </si>
+  <si>
+    <t>San Andreas Landing</t>
+  </si>
+  <si>
+    <t>sal</t>
+  </si>
+  <si>
+    <t>Sacramento R at Rio Vista</t>
+  </si>
+  <si>
+    <t>srv</t>
+  </si>
+  <si>
+    <t>ppt</t>
+  </si>
+  <si>
+    <t>Prisoners Point</t>
+  </si>
+  <si>
+    <t>Old R near Byron</t>
+  </si>
+  <si>
+    <t>oh4</t>
+  </si>
+  <si>
+    <t>hll</t>
+  </si>
+  <si>
+    <t>bet</t>
+  </si>
+  <si>
+    <t>ibs</t>
+  </si>
+  <si>
+    <t>gys</t>
+  </si>
+  <si>
+    <t>Holland Tract</t>
+  </si>
+  <si>
+    <t>Piper Slough at Bethal Tract</t>
+  </si>
+  <si>
+    <t>Cordelia Slough at Ibis club</t>
+  </si>
+  <si>
+    <t>Goodyear Slough at Morrow Island club</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -307,8 +505,23 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -318,6 +531,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor theme="0" tint="-0.14999847407452621"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.499984740745262"/>
         <bgColor theme="0" tint="-0.14999847407452621"/>
       </patternFill>
     </fill>
@@ -354,7 +579,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -371,13 +596,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -388,50 +610,61 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="12">
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
+  <dxfs count="6">
     <dxf>
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -447,6 +680,9 @@
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -461,26 +697,26 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{9F1BA903-751C-4660-B3EA-7CFC748037BB}" name="Table1" displayName="Table1" ref="B1:G37" totalsRowShown="0">
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:G37">
-    <sortCondition ref="C1:C37"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{9F1BA903-751C-4660-B3EA-7CFC748037BB}" name="Table1" displayName="Table1" ref="D1:I37" totalsRowShown="0">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="D2:I37">
+    <sortCondition ref="E1:E37"/>
   </sortState>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{02F85A5B-494A-43D0-A963-65DB30957B18}" name="Description" dataDxfId="6"/>
-    <tableColumn id="2" xr3:uid="{4C7B2D15-6B0D-435B-BB38-D38566CCE77C}" name="SHOULD HAVE FOR CALSIM" dataDxfId="11"/>
-    <tableColumn id="4" xr3:uid="{3986071E-1297-4FE7-9CAE-654E061DDEF2}" name="STRUCTURAL" dataDxfId="10"/>
-    <tableColumn id="5" xr3:uid="{032429B3-7981-42C7-A43E-BD5E70692FDB}" name="??" dataDxfId="9"/>
-    <tableColumn id="3" xr3:uid="{3FD418F8-3AEA-4B06-8D87-70A6F07D7EBF}" name="EXCLUDE" dataDxfId="8"/>
-    <tableColumn id="6" xr3:uid="{5EE2F89F-E9EA-4CFE-84C4-F6B35C503B31}" name="Notes" dataDxfId="7"/>
+    <tableColumn id="1" xr3:uid="{02F85A5B-494A-43D0-A963-65DB30957B18}" name="DSM2 Description" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{4C7B2D15-6B0D-435B-BB38-D38566CCE77C}" name="SHOULD HAVE FOR CALSIM" dataDxfId="4"/>
+    <tableColumn id="4" xr3:uid="{3986071E-1297-4FE7-9CAE-654E061DDEF2}" name="STRUCTURAL" dataDxfId="3"/>
+    <tableColumn id="5" xr3:uid="{032429B3-7981-42C7-A43E-BD5E70692FDB}" name="??" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{3FD418F8-3AEA-4B06-8D87-70A6F07D7EBF}" name="EXCLUDE" dataDxfId="1"/>
+    <tableColumn id="6" xr3:uid="{5EE2F89F-E9EA-4CFE-84C4-F6B35C503B31}" name="Notes" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -518,7 +754,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -624,7 +860,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -766,7 +1002,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -774,625 +1010,837 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B49A5C93-5644-40EC-92F5-9FDA140488D2}">
-  <dimension ref="A1:H37"/>
+  <dimension ref="A1:J38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A24"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18" style="1" customWidth="1"/>
-    <col min="2" max="2" width="54.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="25.85546875" customWidth="1"/>
-    <col min="8" max="8" width="11" style="1" customWidth="1"/>
+    <col min="2" max="2" width="7.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="46" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="54.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="25.85546875" customWidth="1"/>
+    <col min="10" max="10" width="11" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" t="s">
+        <v>83</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="H1"/>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="10" t="s">
+      <c r="J1"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="9" t="s">
         <v>56</v>
       </c>
       <c r="B2" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="D2" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
+      <c r="E2" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="F2" s="1"/>
-      <c r="G2" s="4"/>
-      <c r="H2"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="11" t="s">
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="4"/>
+      <c r="J2"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="B3" s="12" t="s">
+      <c r="B3" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="D3" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
+      <c r="E3" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="F3" s="1"/>
-      <c r="G3" s="4"/>
-      <c r="H3"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="10" t="s">
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="4"/>
+      <c r="J3"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="B4" s="12" t="s">
+      <c r="B4" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="D4" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
+      <c r="E4" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="F4" s="1"/>
-      <c r="G4" s="4"/>
-      <c r="H4"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="11" t="s">
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="4"/>
+      <c r="J4"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="B5" s="12" t="s">
+      <c r="B5" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="C5" s="13" t="s">
+        <v>92</v>
+      </c>
+      <c r="D5" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
+      <c r="E5" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="F5" s="1"/>
-      <c r="G5" s="4"/>
-      <c r="H5"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="10" t="s">
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="4"/>
+      <c r="J5"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="9" t="s">
         <v>65</v>
       </c>
       <c r="B6" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>99</v>
+      </c>
+      <c r="D6" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
+      <c r="E6" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="F6" s="1"/>
-      <c r="G6" s="4"/>
-      <c r="H6"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="11" t="s">
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="4"/>
+      <c r="J6"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="B7" s="9" t="s">
+      <c r="B7" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="C7" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="D7" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
+      <c r="E7" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="F7" s="1"/>
-      <c r="G7" s="4"/>
-      <c r="H7"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="10" t="s">
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="4"/>
+      <c r="J7"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="9" t="s">
         <v>51</v>
       </c>
       <c r="B8" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>102</v>
+      </c>
+      <c r="D8" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
+      <c r="E8" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="F8" s="1"/>
-      <c r="G8" s="4"/>
-      <c r="H8"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="11" t="s">
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="4"/>
+      <c r="J8"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="B9" s="9" t="s">
+      <c r="B9" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="C9" s="13" t="s">
+        <v>106</v>
+      </c>
+      <c r="D9" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
+      <c r="E9" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="F9" s="1"/>
-      <c r="G9" s="4"/>
-      <c r="H9"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="10" t="s">
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="4"/>
+      <c r="J9"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="9" t="s">
         <v>66</v>
       </c>
       <c r="B10" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="C10" s="12" t="s">
+        <v>108</v>
+      </c>
+      <c r="D10" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
+      <c r="E10" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="F10" s="1"/>
-      <c r="G10" s="4"/>
-      <c r="H10"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="8" t="s">
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="4"/>
+      <c r="J10"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="C11" s="14" t="s">
+        <v>130</v>
+      </c>
+      <c r="D11" t="s">
         <v>17</v>
       </c>
-      <c r="C11" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
+      <c r="E11" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="F11" s="1"/>
-      <c r="G11" s="4"/>
-      <c r="H11"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="10" t="s">
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="4"/>
+      <c r="J11"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="9" t="s">
         <v>49</v>
       </c>
       <c r="B12" s="9" t="s">
+        <v>132</v>
+      </c>
+      <c r="C12" s="12" t="s">
+        <v>131</v>
+      </c>
+      <c r="D12" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="C12" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
+      <c r="E12" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="F12" s="1"/>
-      <c r="G12" s="4"/>
-      <c r="H12"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="11" t="s">
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="4"/>
+      <c r="J12"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="B13" s="9" t="s">
+      <c r="B13" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="C13" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="D13" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1" t="s">
-        <v>0</v>
-      </c>
       <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
-      <c r="G13" s="4"/>
-      <c r="H13"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="10" t="s">
+      <c r="F13" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="4"/>
+      <c r="J13"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" s="9" t="s">
         <v>70</v>
       </c>
       <c r="B14" s="9" t="s">
+        <v>134</v>
+      </c>
+      <c r="C14" s="12" t="s">
+        <v>133</v>
+      </c>
+      <c r="D14" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1" t="s">
-        <v>0</v>
-      </c>
       <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
-      <c r="G14" s="4"/>
-      <c r="H14"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="11" t="s">
+      <c r="F14" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="4"/>
+      <c r="J14"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="B15" s="9" t="s">
+      <c r="B15" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="C15" s="13" t="s">
+        <v>104</v>
+      </c>
+      <c r="D15" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1" t="s">
-        <v>0</v>
-      </c>
       <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
-      <c r="G15" s="4"/>
-      <c r="H15"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="10" t="s">
+      <c r="F15" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="4"/>
+      <c r="J15"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" s="9" t="s">
         <v>50</v>
       </c>
       <c r="B16" s="9" t="s">
+        <v>135</v>
+      </c>
+      <c r="C16" s="12" t="s">
+        <v>136</v>
+      </c>
+      <c r="D16" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1" t="s">
-        <v>0</v>
-      </c>
       <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
-      <c r="G16" s="4"/>
-      <c r="H16"/>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="11" t="s">
+      <c r="F16" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
+      <c r="I16" s="4"/>
+      <c r="J16"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="B17" s="9" t="s">
+      <c r="B17" s="10" t="s">
+        <v>118</v>
+      </c>
+      <c r="C17" s="13" t="s">
+        <v>117</v>
+      </c>
+      <c r="D17" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1" t="s">
-        <v>0</v>
-      </c>
       <c r="E17" s="1"/>
-      <c r="F17" s="1"/>
-      <c r="G17" s="4"/>
-      <c r="H17"/>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="10" t="s">
+      <c r="F17" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
+      <c r="I17" s="4"/>
+      <c r="J17"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" s="9" t="s">
         <v>64</v>
       </c>
       <c r="B18" s="9" t="s">
+        <v>120</v>
+      </c>
+      <c r="C18" s="12" t="s">
+        <v>119</v>
+      </c>
+      <c r="D18" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="C18" s="1"/>
-      <c r="D18" s="1" t="s">
-        <v>0</v>
-      </c>
       <c r="E18" s="1"/>
-      <c r="F18" s="1"/>
-      <c r="G18" s="4"/>
-      <c r="H18"/>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="11" t="s">
+      <c r="F18" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
+      <c r="I18" s="4"/>
+      <c r="J18"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="B19" s="9" t="s">
+      <c r="B19" s="10" t="s">
+        <v>121</v>
+      </c>
+      <c r="C19" s="13" t="s">
+        <v>122</v>
+      </c>
+      <c r="D19" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1" t="s">
-        <v>0</v>
-      </c>
       <c r="E19" s="1"/>
-      <c r="F19" s="1"/>
-      <c r="G19" s="4"/>
-      <c r="H19"/>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="7" t="s">
+      <c r="F19" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G19" s="1"/>
+      <c r="H19" s="1"/>
+      <c r="I19" s="4"/>
+      <c r="J19"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="6" t="s">
+        <v>138</v>
+      </c>
+      <c r="C20" s="15" t="s">
+        <v>137</v>
+      </c>
+      <c r="D20" t="s">
         <v>26</v>
       </c>
-      <c r="C20" s="1"/>
-      <c r="D20" s="1" t="s">
-        <v>0</v>
-      </c>
       <c r="E20" s="1"/>
-      <c r="F20" s="1"/>
-      <c r="G20" s="4"/>
-      <c r="H20"/>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="8" t="s">
+      <c r="F20" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G20" s="1"/>
+      <c r="H20" s="1"/>
+      <c r="I20" s="4"/>
+      <c r="J20"/>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="C21" s="14" t="s">
+        <v>143</v>
+      </c>
+      <c r="D21" t="s">
         <v>27</v>
       </c>
-      <c r="C21" s="1"/>
-      <c r="D21" s="1" t="s">
-        <v>0</v>
-      </c>
       <c r="E21" s="1"/>
-      <c r="F21" s="1"/>
-      <c r="G21" s="4"/>
-      <c r="H21"/>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="7" t="s">
+      <c r="F21" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G21" s="1"/>
+      <c r="H21" s="1"/>
+      <c r="I21" s="4"/>
+      <c r="J21"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" s="6" t="s">
+        <v>140</v>
+      </c>
+      <c r="C22" s="15" t="s">
+        <v>144</v>
+      </c>
+      <c r="D22" t="s">
         <v>28</v>
       </c>
-      <c r="C22" s="1"/>
-      <c r="D22" s="1" t="s">
-        <v>0</v>
-      </c>
       <c r="E22" s="1"/>
-      <c r="F22" s="1"/>
-      <c r="G22" s="4"/>
-      <c r="H22"/>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="8" t="s">
+      <c r="F22" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G22" s="1"/>
+      <c r="H22" s="1"/>
+      <c r="I22" s="4"/>
+      <c r="J22"/>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B23" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="C23" s="14" t="s">
+        <v>145</v>
+      </c>
+      <c r="D23" t="s">
         <v>29</v>
       </c>
-      <c r="C23" s="1"/>
-      <c r="D23" s="1" t="s">
-        <v>0</v>
-      </c>
       <c r="E23" s="1"/>
-      <c r="F23" s="1"/>
-      <c r="G23" s="4"/>
-      <c r="H23"/>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="7" t="s">
+      <c r="F23" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G23" s="1"/>
+      <c r="H23" s="1"/>
+      <c r="I23" s="4"/>
+      <c r="J23"/>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A24" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B24" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="C24" s="15" t="s">
+        <v>146</v>
+      </c>
+      <c r="D24" t="s">
         <v>30</v>
       </c>
-      <c r="C24" s="1"/>
-      <c r="D24" s="1" t="s">
-        <v>0</v>
-      </c>
       <c r="E24" s="1"/>
-      <c r="F24" s="1"/>
-      <c r="G24" s="4"/>
-      <c r="H24"/>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="11" t="s">
+      <c r="F24" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G24" s="1"/>
+      <c r="H24" s="1"/>
+      <c r="I24" s="4"/>
+      <c r="J24"/>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A25" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="B25" s="9" t="s">
+      <c r="B25" s="16" t="s">
+        <v>123</v>
+      </c>
+      <c r="C25" s="17" t="s">
+        <v>125</v>
+      </c>
+      <c r="D25" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="C25" s="1"/>
-      <c r="D25" s="1"/>
-      <c r="E25" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="F25" s="1"/>
-      <c r="G25" s="4" t="s">
+      <c r="E25" s="19"/>
+      <c r="F25" s="19"/>
+      <c r="G25" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="H25" s="19"/>
+      <c r="I25" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="H25"/>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="7" t="s">
+      <c r="J25"/>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A26" s="21" t="s">
         <v>76</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B26" s="21"/>
+      <c r="C26" s="22"/>
+      <c r="D26" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
-      <c r="E26" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="F26" s="1"/>
-      <c r="G26" s="4"/>
-      <c r="H26"/>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="8" t="s">
+      <c r="E26" s="19"/>
+      <c r="F26" s="19"/>
+      <c r="G26" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="H26" s="19"/>
+      <c r="I26" s="20"/>
+      <c r="J26"/>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A27" s="24" t="s">
         <v>77</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B27" s="24"/>
+      <c r="C27" s="25"/>
+      <c r="D27" s="23" t="s">
         <v>33</v>
       </c>
-      <c r="C27" s="1"/>
-      <c r="D27" s="1"/>
-      <c r="E27" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="F27" s="1"/>
-      <c r="G27" s="4"/>
-      <c r="H27"/>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="10" t="s">
+      <c r="E27" s="19"/>
+      <c r="F27" s="19"/>
+      <c r="G27" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="H27" s="19"/>
+      <c r="I27" s="20"/>
+      <c r="J27"/>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A28" s="26" t="s">
         <v>61</v>
       </c>
-      <c r="B28" s="9" t="s">
+      <c r="B28" s="26" t="s">
+        <v>93</v>
+      </c>
+      <c r="C28" s="27" t="s">
+        <v>94</v>
+      </c>
+      <c r="D28" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="C28" s="1"/>
-      <c r="D28" s="1"/>
-      <c r="E28" s="1"/>
-      <c r="F28" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="G28" s="4"/>
-      <c r="H28"/>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" s="8" t="s">
+      <c r="E28" s="19"/>
+      <c r="F28" s="19"/>
+      <c r="G28" s="19"/>
+      <c r="H28" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="I28" s="20"/>
+      <c r="J28"/>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A29" s="24" t="s">
         <v>78</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B29" s="24" t="s">
+        <v>124</v>
+      </c>
+      <c r="C29" s="25" t="s">
+        <v>126</v>
+      </c>
+      <c r="D29" s="23" t="s">
         <v>35</v>
       </c>
-      <c r="C29" s="1"/>
-      <c r="D29" s="1"/>
-      <c r="E29" s="1"/>
-      <c r="F29" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="G29" s="4"/>
-      <c r="H29"/>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" s="7" t="s">
+      <c r="E29" s="19"/>
+      <c r="F29" s="19"/>
+      <c r="G29" s="19"/>
+      <c r="H29" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="I29" s="20"/>
+      <c r="J29"/>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A30" s="21" t="s">
         <v>79</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B30" s="21"/>
+      <c r="C30" s="22"/>
+      <c r="D30" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="C30" s="1"/>
-      <c r="D30" s="1"/>
-      <c r="E30" s="1"/>
-      <c r="F30" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="G30" s="4"/>
-      <c r="H30"/>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" s="8" t="s">
+      <c r="E30" s="19"/>
+      <c r="F30" s="19"/>
+      <c r="G30" s="19"/>
+      <c r="H30" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="I30" s="20"/>
+      <c r="J30"/>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A31" s="24" t="s">
         <v>47</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B31" s="24"/>
+      <c r="C31" s="25"/>
+      <c r="D31" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="C31" s="1"/>
-      <c r="D31" s="1"/>
-      <c r="E31" s="1"/>
-      <c r="F31" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="G31" s="4"/>
-      <c r="H31"/>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32" s="10" t="s">
+      <c r="E31" s="19"/>
+      <c r="F31" s="19"/>
+      <c r="G31" s="19"/>
+      <c r="H31" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="I31" s="20"/>
+      <c r="J31"/>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A32" s="26" t="s">
         <v>59</v>
       </c>
-      <c r="B32" s="9" t="s">
+      <c r="B32" s="26" t="s">
+        <v>89</v>
+      </c>
+      <c r="C32" s="27" t="s">
+        <v>90</v>
+      </c>
+      <c r="D32" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="C32" s="1"/>
-      <c r="D32" s="1"/>
-      <c r="E32" s="1"/>
-      <c r="F32" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="G32" s="4"/>
-      <c r="H32"/>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A33" s="11" t="s">
+      <c r="E32" s="19"/>
+      <c r="F32" s="19"/>
+      <c r="G32" s="19"/>
+      <c r="H32" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="I32" s="20"/>
+      <c r="J32"/>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A33" s="16" t="s">
         <v>60</v>
       </c>
-      <c r="B33" s="9" t="s">
+      <c r="B33" s="16" t="s">
+        <v>110</v>
+      </c>
+      <c r="C33" s="17" t="s">
+        <v>109</v>
+      </c>
+      <c r="D33" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="C33" s="1"/>
-      <c r="D33" s="1"/>
-      <c r="E33" s="1"/>
-      <c r="F33" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="G33" s="4"/>
-      <c r="H33"/>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A34" s="10" t="s">
+      <c r="E33" s="19"/>
+      <c r="F33" s="19"/>
+      <c r="G33" s="19"/>
+      <c r="H33" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="I33" s="20"/>
+      <c r="J33"/>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A34" s="26" t="s">
         <v>58</v>
       </c>
-      <c r="B34" s="9" t="s">
+      <c r="B34" s="26" t="s">
+        <v>112</v>
+      </c>
+      <c r="C34" s="27" t="s">
+        <v>111</v>
+      </c>
+      <c r="D34" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="C34" s="1"/>
-      <c r="D34" s="1"/>
-      <c r="E34" s="1"/>
-      <c r="F34" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="G34" s="4"/>
-      <c r="H34"/>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A35" s="11" t="s">
+      <c r="E34" s="19"/>
+      <c r="F34" s="19"/>
+      <c r="G34" s="19"/>
+      <c r="H34" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="I34" s="20"/>
+      <c r="J34"/>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A35" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="B35" s="9" t="s">
+      <c r="B35" s="16" t="s">
+        <v>116</v>
+      </c>
+      <c r="C35" s="17" t="s">
+        <v>115</v>
+      </c>
+      <c r="D35" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="C35" s="1"/>
-      <c r="D35" s="1"/>
-      <c r="E35" s="1"/>
-      <c r="F35" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="G35" s="4"/>
-      <c r="H35"/>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A36" s="10" t="s">
+      <c r="E35" s="19"/>
+      <c r="F35" s="19"/>
+      <c r="G35" s="19"/>
+      <c r="H35" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="I35" s="20"/>
+      <c r="J35"/>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A36" s="26" t="s">
         <v>68</v>
       </c>
-      <c r="B36" s="9" t="s">
+      <c r="B36" s="26" t="s">
+        <v>114</v>
+      </c>
+      <c r="C36" s="27" t="s">
+        <v>113</v>
+      </c>
+      <c r="D36" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="C36" s="1"/>
-      <c r="D36" s="1"/>
-      <c r="E36" s="1"/>
-      <c r="F36" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="G36" s="4"/>
-      <c r="H36"/>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A37" s="6" t="s">
+      <c r="E36" s="19"/>
+      <c r="F36" s="19"/>
+      <c r="G36" s="19"/>
+      <c r="H36" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="I36" s="20"/>
+      <c r="J36"/>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A37" s="28" t="s">
         <v>80</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B37" s="28"/>
+      <c r="C37" s="29"/>
+      <c r="D37" s="23" t="s">
         <v>43</v>
       </c>
-      <c r="C37" s="1"/>
-      <c r="D37" s="1"/>
-      <c r="E37" s="1"/>
-      <c r="F37" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="G37" s="4"/>
-      <c r="H37"/>
+      <c r="E37" s="19"/>
+      <c r="F37" s="19"/>
+      <c r="G37" s="19"/>
+      <c r="H37" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="I37" s="20"/>
+      <c r="J37"/>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B38" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>128</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>

<commit_message>
fixed stations per convo w Eli
</commit_message>
<xml_diff>
--- a/data/Stations_Importance.xlsx
+++ b/data/Stations_Importance.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\delta_salinity\scripts\DSP_code\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46B99664-A13E-4C88-B1D7-E28FFE933137}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D42BBCAA-B560-4514-A2B1-9F9C2ADCF50A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28800" yWindow="0" windowWidth="14400" windowHeight="17550" xr2:uid="{DB7A9B06-FD48-4539-AA38-6D28440ECAB7}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17790" xr2:uid="{DB7A9B06-FD48-4539-AA38-6D28440ECAB7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="150">
   <si>
     <t>Y</t>
   </si>
@@ -290,9 +290,6 @@
     <t>DSM2 Description</t>
   </si>
   <si>
-    <t>CBP Intake at Tracy Pumping Plant</t>
-  </si>
-  <si>
     <t>wci</t>
   </si>
   <si>
@@ -311,9 +308,6 @@
     <t>Old River neart Middle River</t>
   </si>
   <si>
-    <t>obi</t>
-  </si>
-  <si>
     <t>Old R at Bacon Island</t>
   </si>
   <si>
@@ -338,18 +332,9 @@
     <t>Sacramento River at Mallard Island</t>
   </si>
   <si>
-    <t>cse</t>
-  </si>
-  <si>
-    <t>emm2</t>
-  </si>
-  <si>
     <t>Sacramento River at Emmaton</t>
   </si>
   <si>
-    <t>anh</t>
-  </si>
-  <si>
     <t>San Joaquin at Antioch</t>
   </si>
   <si>
@@ -398,9 +383,6 @@
     <t>Montezuma Slough at National Steel</t>
   </si>
   <si>
-    <t>nsl2</t>
-  </si>
-  <si>
     <t>vol</t>
   </si>
   <si>
@@ -477,6 +459,33 @@
   </si>
   <si>
     <t>Goodyear Slough at Morrow Island club</t>
+  </si>
+  <si>
+    <t>not in DSM2</t>
+  </si>
+  <si>
+    <t>CVP Intake at Tracy Pumping Plant</t>
+  </si>
+  <si>
+    <t>bac</t>
+  </si>
+  <si>
+    <t>cll</t>
+  </si>
+  <si>
+    <t>emm</t>
+  </si>
+  <si>
+    <t>anc</t>
+  </si>
+  <si>
+    <t>nsl</t>
+  </si>
+  <si>
+    <t>tms</t>
+  </si>
+  <si>
+    <t>Threemile Slough near Rio Vista</t>
   </si>
 </sst>
 </file>
@@ -596,9 +605,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -619,9 +625,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -660,6 +663,8 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -697,9 +702,9 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{9F1BA903-751C-4660-B3EA-7CFC748037BB}" name="Table1" displayName="Table1" ref="D1:I37" totalsRowShown="0">
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="D2:I37">
-    <sortCondition ref="E1:E37"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{9F1BA903-751C-4660-B3EA-7CFC748037BB}" name="Table1" displayName="Table1" ref="D1:I39" totalsRowShown="0">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="D2:I38">
+    <sortCondition ref="E1:E38"/>
   </sortState>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{02F85A5B-494A-43D0-A963-65DB30957B18}" name="DSM2 Description" dataDxfId="5"/>
@@ -1010,10 +1015,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B49A5C93-5644-40EC-92F5-9FDA140488D2}">
-  <dimension ref="A1:J38"/>
+  <dimension ref="A1:J39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="I26" sqref="A26:I39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1061,16 +1066,16 @@
       <c r="J1"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="C2" s="12" t="s">
-        <v>84</v>
-      </c>
-      <c r="D2" s="8" t="s">
+      <c r="C2" s="11" t="s">
+        <v>142</v>
+      </c>
+      <c r="D2" s="7" t="s">
         <v>8</v>
       </c>
       <c r="E2" s="1" t="s">
@@ -1083,16 +1088,16 @@
       <c r="J2"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="10" t="s">
+      <c r="A3" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="C3" s="12" t="s">
         <v>85</v>
       </c>
-      <c r="C3" s="13" t="s">
-        <v>86</v>
-      </c>
-      <c r="D3" s="11" t="s">
+      <c r="D3" s="10" t="s">
         <v>9</v>
       </c>
       <c r="E3" s="1" t="s">
@@ -1105,16 +1110,16 @@
       <c r="J3"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="C4" s="11" t="s">
         <v>87</v>
       </c>
-      <c r="C4" s="12" t="s">
-        <v>88</v>
-      </c>
-      <c r="D4" s="11" t="s">
+      <c r="D4" s="10" t="s">
         <v>10</v>
       </c>
       <c r="E4" s="1" t="s">
@@ -1127,16 +1132,16 @@
       <c r="J4"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="10" t="s">
+      <c r="A5" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="B5" s="10" t="s">
-        <v>91</v>
-      </c>
-      <c r="C5" s="13" t="s">
-        <v>92</v>
-      </c>
-      <c r="D5" s="11" t="s">
+      <c r="B5" s="9" t="s">
+        <v>143</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="D5" s="10" t="s">
         <v>11</v>
       </c>
       <c r="E5" s="1" t="s">
@@ -1149,16 +1154,16 @@
       <c r="J5"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="9" t="s">
+      <c r="A6" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="C6" s="11" t="s">
         <v>97</v>
       </c>
-      <c r="C6" s="12" t="s">
-        <v>99</v>
-      </c>
-      <c r="D6" s="8" t="s">
+      <c r="D6" s="7" t="s">
         <v>12</v>
       </c>
       <c r="E6" s="1" t="s">
@@ -1171,16 +1176,16 @@
       <c r="J6"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="10" t="s">
+      <c r="A7" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="B7" s="10" t="s">
-        <v>100</v>
-      </c>
-      <c r="C7" s="13" t="s">
-        <v>98</v>
-      </c>
-      <c r="D7" s="8" t="s">
+      <c r="B7" s="9" t="s">
+        <v>144</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>96</v>
+      </c>
+      <c r="D7" s="7" t="s">
         <v>13</v>
       </c>
       <c r="E7" s="1" t="s">
@@ -1193,16 +1198,16 @@
       <c r="J7"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="9" t="s">
+      <c r="A8" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="B8" s="9" t="s">
-        <v>101</v>
-      </c>
-      <c r="C8" s="12" t="s">
-        <v>102</v>
-      </c>
-      <c r="D8" s="8" t="s">
+      <c r="B8" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="D8" s="7" t="s">
         <v>14</v>
       </c>
       <c r="E8" s="1" t="s">
@@ -1215,16 +1220,16 @@
       <c r="J8"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="10" t="s">
+      <c r="A9" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="B9" s="10" t="s">
-        <v>105</v>
-      </c>
-      <c r="C9" s="13" t="s">
-        <v>106</v>
-      </c>
-      <c r="D9" s="8" t="s">
+      <c r="B9" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="C9" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="D9" s="7" t="s">
         <v>15</v>
       </c>
       <c r="E9" s="1" t="s">
@@ -1237,16 +1242,16 @@
       <c r="J9"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="9" t="s">
+      <c r="A10" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="B10" s="9" t="s">
-        <v>107</v>
-      </c>
-      <c r="C10" s="12" t="s">
-        <v>108</v>
-      </c>
-      <c r="D10" s="8" t="s">
+      <c r="B10" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="D10" s="7" t="s">
         <v>16</v>
       </c>
       <c r="E10" s="1" t="s">
@@ -1259,14 +1264,14 @@
       <c r="J10"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="7" t="s">
+      <c r="A11" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="B11" s="7" t="s">
-        <v>129</v>
-      </c>
-      <c r="C11" s="14" t="s">
-        <v>130</v>
+      <c r="B11" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="C11" s="13" t="s">
+        <v>124</v>
       </c>
       <c r="D11" t="s">
         <v>17</v>
@@ -1281,16 +1286,16 @@
       <c r="J11"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="9" t="s">
+      <c r="A12" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="B12" s="9" t="s">
-        <v>132</v>
-      </c>
-      <c r="C12" s="12" t="s">
-        <v>131</v>
-      </c>
-      <c r="D12" s="8" t="s">
+      <c r="B12" s="8" t="s">
+        <v>126</v>
+      </c>
+      <c r="C12" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="D12" s="7" t="s">
         <v>18</v>
       </c>
       <c r="E12" s="1" t="s">
@@ -1303,39 +1308,35 @@
       <c r="J12"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="B13" s="10" t="s">
-        <v>96</v>
+      <c r="A13" s="6"/>
+      <c r="B13" s="6" t="s">
+        <v>148</v>
       </c>
       <c r="C13" s="13" t="s">
-        <v>95</v>
-      </c>
-      <c r="D13" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1" t="s">
-        <v>0</v>
-      </c>
+        <v>149</v>
+      </c>
+      <c r="D13" s="29"/>
+      <c r="E13" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F13" s="1"/>
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
       <c r="I13" s="4"/>
       <c r="J13"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="9" t="s">
-        <v>70</v>
-      </c>
-      <c r="B14" s="9" t="s">
-        <v>134</v>
-      </c>
-      <c r="C14" s="12" t="s">
-        <v>133</v>
-      </c>
-      <c r="D14" s="8" t="s">
-        <v>20</v>
+      <c r="A14" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="C14" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>19</v>
       </c>
       <c r="E14" s="1"/>
       <c r="F14" s="1" t="s">
@@ -1347,17 +1348,17 @@
       <c r="J14"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="10" t="s">
-        <v>62</v>
-      </c>
-      <c r="B15" s="10" t="s">
-        <v>103</v>
-      </c>
-      <c r="C15" s="13" t="s">
-        <v>104</v>
-      </c>
-      <c r="D15" s="8" t="s">
-        <v>21</v>
+      <c r="A15" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>128</v>
+      </c>
+      <c r="C15" s="12" t="s">
+        <v>127</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>20</v>
       </c>
       <c r="E15" s="1"/>
       <c r="F15" s="1" t="s">
@@ -1369,17 +1370,17 @@
       <c r="J15"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="B16" s="9" t="s">
-        <v>135</v>
-      </c>
-      <c r="C16" s="12" t="s">
-        <v>136</v>
-      </c>
-      <c r="D16" s="8" t="s">
-        <v>22</v>
+      <c r="A16" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>146</v>
+      </c>
+      <c r="C16" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>21</v>
       </c>
       <c r="E16" s="1"/>
       <c r="F16" s="1" t="s">
@@ -1391,17 +1392,17 @@
       <c r="J16"/>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="B17" s="10" t="s">
-        <v>118</v>
+      <c r="A17" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>129</v>
       </c>
       <c r="C17" s="13" t="s">
-        <v>117</v>
-      </c>
-      <c r="D17" s="8" t="s">
-        <v>23</v>
+        <v>130</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>22</v>
       </c>
       <c r="E17" s="1"/>
       <c r="F17" s="1" t="s">
@@ -1413,17 +1414,17 @@
       <c r="J17"/>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" s="9" t="s">
-        <v>64</v>
-      </c>
-      <c r="B18" s="9" t="s">
-        <v>120</v>
-      </c>
-      <c r="C18" s="12" t="s">
-        <v>119</v>
-      </c>
-      <c r="D18" s="8" t="s">
-        <v>24</v>
+      <c r="A18" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="B18" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="C18" s="11" t="s">
+        <v>112</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>23</v>
       </c>
       <c r="E18" s="1"/>
       <c r="F18" s="1" t="s">
@@ -1435,17 +1436,17 @@
       <c r="J18"/>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" s="10" t="s">
-        <v>67</v>
-      </c>
-      <c r="B19" s="10" t="s">
-        <v>121</v>
-      </c>
-      <c r="C19" s="13" t="s">
-        <v>122</v>
-      </c>
-      <c r="D19" s="8" t="s">
-        <v>25</v>
+      <c r="A19" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="B19" s="9" t="s">
+        <v>147</v>
+      </c>
+      <c r="C19" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="D19" s="7" t="s">
+        <v>24</v>
       </c>
       <c r="E19" s="1"/>
       <c r="F19" s="1" t="s">
@@ -1457,17 +1458,17 @@
       <c r="J19"/>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="B20" s="6" t="s">
-        <v>138</v>
-      </c>
-      <c r="C20" s="15" t="s">
-        <v>137</v>
-      </c>
-      <c r="D20" t="s">
-        <v>26</v>
+      <c r="A20" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="B20" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="C20" s="11" t="s">
+        <v>116</v>
+      </c>
+      <c r="D20" s="7" t="s">
+        <v>25</v>
       </c>
       <c r="E20" s="1"/>
       <c r="F20" s="1" t="s">
@@ -1479,17 +1480,17 @@
       <c r="J20"/>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A21" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="B21" s="7" t="s">
-        <v>139</v>
-      </c>
-      <c r="C21" s="14" t="s">
-        <v>143</v>
+      <c r="A21" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="C21" s="13" t="s">
+        <v>131</v>
       </c>
       <c r="D21" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E21" s="1"/>
       <c r="F21" s="1" t="s">
@@ -1501,17 +1502,17 @@
       <c r="J21"/>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="B22" s="6" t="s">
-        <v>140</v>
-      </c>
-      <c r="C22" s="15" t="s">
-        <v>144</v>
+      <c r="A22" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="B22" s="8" t="s">
+        <v>133</v>
+      </c>
+      <c r="C22" s="11" t="s">
+        <v>137</v>
       </c>
       <c r="D22" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E22" s="1"/>
       <c r="F22" s="1" t="s">
@@ -1523,17 +1524,17 @@
       <c r="J22"/>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A23" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="B23" s="7" t="s">
-        <v>141</v>
-      </c>
-      <c r="C23" s="14" t="s">
-        <v>145</v>
+      <c r="A23" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="B23" s="9" t="s">
+        <v>134</v>
+      </c>
+      <c r="C23" s="12" t="s">
+        <v>138</v>
       </c>
       <c r="D23" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E23" s="1"/>
       <c r="F23" s="1" t="s">
@@ -1545,17 +1546,17 @@
       <c r="J23"/>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A24" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="B24" s="6" t="s">
-        <v>142</v>
-      </c>
-      <c r="C24" s="15" t="s">
-        <v>146</v>
+      <c r="A24" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="B24" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="C24" s="11" t="s">
+        <v>139</v>
       </c>
       <c r="D24" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E24" s="1"/>
       <c r="F24" s="1" t="s">
@@ -1567,279 +1568,309 @@
       <c r="J24"/>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A25" s="16" t="s">
+      <c r="A25" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="B25" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="C25" s="13" t="s">
+        <v>140</v>
+      </c>
+      <c r="D25" t="s">
+        <v>30</v>
+      </c>
+      <c r="E25" s="1"/>
+      <c r="F25" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G25" s="1"/>
+      <c r="H25" s="1"/>
+      <c r="I25" s="4"/>
+      <c r="J25"/>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A26" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="B25" s="16" t="s">
-        <v>123</v>
-      </c>
-      <c r="C25" s="17" t="s">
-        <v>125</v>
-      </c>
-      <c r="D25" s="18" t="s">
+      <c r="B26" s="14" t="s">
+        <v>117</v>
+      </c>
+      <c r="C26" s="15" t="s">
+        <v>119</v>
+      </c>
+      <c r="D26" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="E25" s="19"/>
-      <c r="F25" s="19"/>
-      <c r="G25" s="19" t="s">
-        <v>0</v>
-      </c>
-      <c r="H25" s="19"/>
-      <c r="I25" s="20" t="s">
+      <c r="E26" s="17"/>
+      <c r="F26" s="17"/>
+      <c r="G26" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="H26" s="17"/>
+      <c r="I26" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="J25"/>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A26" s="21" t="s">
+      <c r="J26"/>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A27" s="19" t="s">
         <v>76</v>
       </c>
-      <c r="B26" s="21"/>
-      <c r="C26" s="22"/>
-      <c r="D26" s="23" t="s">
+      <c r="B27" s="19"/>
+      <c r="C27" s="20"/>
+      <c r="D27" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="E26" s="19"/>
-      <c r="F26" s="19"/>
-      <c r="G26" s="19" t="s">
-        <v>0</v>
-      </c>
-      <c r="H26" s="19"/>
-      <c r="I26" s="20"/>
-      <c r="J26"/>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A27" s="24" t="s">
+      <c r="E27" s="17"/>
+      <c r="F27" s="17"/>
+      <c r="G27" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="H27" s="17"/>
+      <c r="I27" s="18"/>
+      <c r="J27"/>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A28" s="22" t="s">
         <v>77</v>
       </c>
-      <c r="B27" s="24"/>
-      <c r="C27" s="25"/>
-      <c r="D27" s="23" t="s">
+      <c r="B28" s="22"/>
+      <c r="C28" s="23"/>
+      <c r="D28" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="E27" s="19"/>
-      <c r="F27" s="19"/>
-      <c r="G27" s="19" t="s">
-        <v>0</v>
-      </c>
-      <c r="H27" s="19"/>
-      <c r="I27" s="20"/>
-      <c r="J27"/>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A28" s="26" t="s">
-        <v>61</v>
-      </c>
-      <c r="B28" s="26" t="s">
-        <v>93</v>
-      </c>
-      <c r="C28" s="27" t="s">
-        <v>94</v>
-      </c>
-      <c r="D28" s="18" t="s">
-        <v>34</v>
-      </c>
-      <c r="E28" s="19"/>
-      <c r="F28" s="19"/>
-      <c r="G28" s="19"/>
-      <c r="H28" s="19" t="s">
-        <v>0</v>
-      </c>
-      <c r="I28" s="20"/>
+      <c r="E28" s="17"/>
+      <c r="F28" s="17"/>
+      <c r="G28" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="H28" s="17"/>
+      <c r="I28" s="18"/>
       <c r="J28"/>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="24" t="s">
+        <v>61</v>
+      </c>
+      <c r="B29" s="24" t="s">
+        <v>91</v>
+      </c>
+      <c r="C29" s="25" t="s">
+        <v>92</v>
+      </c>
+      <c r="D29" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="E29" s="17"/>
+      <c r="F29" s="17"/>
+      <c r="G29" s="17"/>
+      <c r="H29" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="I29" s="18"/>
+      <c r="J29"/>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A30" s="22" t="s">
         <v>78</v>
       </c>
-      <c r="B29" s="24" t="s">
-        <v>124</v>
-      </c>
-      <c r="C29" s="25" t="s">
-        <v>126</v>
-      </c>
-      <c r="D29" s="23" t="s">
+      <c r="B30" s="22" t="s">
+        <v>118</v>
+      </c>
+      <c r="C30" s="23" t="s">
+        <v>120</v>
+      </c>
+      <c r="D30" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="E29" s="19"/>
-      <c r="F29" s="19"/>
-      <c r="G29" s="19"/>
-      <c r="H29" s="19" t="s">
-        <v>0</v>
-      </c>
-      <c r="I29" s="20"/>
-      <c r="J29"/>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A30" s="21" t="s">
+      <c r="E30" s="17"/>
+      <c r="F30" s="17"/>
+      <c r="G30" s="17"/>
+      <c r="H30" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="I30" s="18"/>
+      <c r="J30"/>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A31" s="19" t="s">
         <v>79</v>
       </c>
-      <c r="B30" s="21"/>
-      <c r="C30" s="22"/>
-      <c r="D30" s="23" t="s">
+      <c r="B31" s="19"/>
+      <c r="C31" s="20"/>
+      <c r="D31" s="21" t="s">
         <v>36</v>
       </c>
-      <c r="E30" s="19"/>
-      <c r="F30" s="19"/>
-      <c r="G30" s="19"/>
-      <c r="H30" s="19" t="s">
-        <v>0</v>
-      </c>
-      <c r="I30" s="20"/>
-      <c r="J30"/>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A31" s="24" t="s">
+      <c r="E31" s="17"/>
+      <c r="F31" s="17"/>
+      <c r="G31" s="17"/>
+      <c r="H31" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="I31" s="18"/>
+      <c r="J31"/>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A32" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="B31" s="24"/>
-      <c r="C31" s="25"/>
-      <c r="D31" s="23" t="s">
+      <c r="B32" s="22"/>
+      <c r="C32" s="23"/>
+      <c r="D32" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="E31" s="19"/>
-      <c r="F31" s="19"/>
-      <c r="G31" s="19"/>
-      <c r="H31" s="19" t="s">
-        <v>0</v>
-      </c>
-      <c r="I31" s="20"/>
-      <c r="J31"/>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A32" s="26" t="s">
+      <c r="E32" s="17"/>
+      <c r="F32" s="17"/>
+      <c r="G32" s="17"/>
+      <c r="H32" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="I32" s="18"/>
+      <c r="J32"/>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A33" s="24" t="s">
         <v>59</v>
       </c>
-      <c r="B32" s="26" t="s">
+      <c r="B33" s="24" t="s">
+        <v>88</v>
+      </c>
+      <c r="C33" s="25" t="s">
         <v>89</v>
       </c>
-      <c r="C32" s="27" t="s">
-        <v>90</v>
-      </c>
-      <c r="D32" s="18" t="s">
+      <c r="D33" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="E32" s="19"/>
-      <c r="F32" s="19"/>
-      <c r="G32" s="19"/>
-      <c r="H32" s="19" t="s">
-        <v>0</v>
-      </c>
-      <c r="I32" s="20"/>
-      <c r="J32"/>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A33" s="16" t="s">
+      <c r="E33" s="17"/>
+      <c r="F33" s="17"/>
+      <c r="G33" s="17"/>
+      <c r="H33" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="I33" s="18"/>
+      <c r="J33"/>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A34" s="14" t="s">
         <v>60</v>
       </c>
-      <c r="B33" s="16" t="s">
+      <c r="B34" s="14" t="s">
+        <v>105</v>
+      </c>
+      <c r="C34" s="15" t="s">
+        <v>104</v>
+      </c>
+      <c r="D34" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="E34" s="17"/>
+      <c r="F34" s="17"/>
+      <c r="G34" s="17"/>
+      <c r="H34" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="I34" s="18"/>
+      <c r="J34"/>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A35" s="24" t="s">
+        <v>58</v>
+      </c>
+      <c r="B35" s="24" t="s">
+        <v>107</v>
+      </c>
+      <c r="C35" s="25" t="s">
+        <v>106</v>
+      </c>
+      <c r="D35" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="E35" s="17"/>
+      <c r="F35" s="17"/>
+      <c r="G35" s="17"/>
+      <c r="H35" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="I35" s="18"/>
+      <c r="J35"/>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A36" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="B36" s="14" t="s">
+        <v>111</v>
+      </c>
+      <c r="C36" s="15" t="s">
         <v>110</v>
       </c>
-      <c r="C33" s="17" t="s">
+      <c r="D36" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="E36" s="17"/>
+      <c r="F36" s="17"/>
+      <c r="G36" s="17"/>
+      <c r="H36" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="I36" s="18"/>
+      <c r="J36"/>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A37" s="24" t="s">
+        <v>68</v>
+      </c>
+      <c r="B37" s="24" t="s">
         <v>109</v>
       </c>
-      <c r="D33" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="E33" s="19"/>
-      <c r="F33" s="19"/>
-      <c r="G33" s="19"/>
-      <c r="H33" s="19" t="s">
-        <v>0</v>
-      </c>
-      <c r="I33" s="20"/>
-      <c r="J33"/>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A34" s="26" t="s">
-        <v>58</v>
-      </c>
-      <c r="B34" s="26" t="s">
-        <v>112</v>
-      </c>
-      <c r="C34" s="27" t="s">
-        <v>111</v>
-      </c>
-      <c r="D34" s="18" t="s">
-        <v>40</v>
-      </c>
-      <c r="E34" s="19"/>
-      <c r="F34" s="19"/>
-      <c r="G34" s="19"/>
-      <c r="H34" s="19" t="s">
-        <v>0</v>
-      </c>
-      <c r="I34" s="20"/>
-      <c r="J34"/>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A35" s="16" t="s">
-        <v>48</v>
-      </c>
-      <c r="B35" s="16" t="s">
-        <v>116</v>
-      </c>
-      <c r="C35" s="17" t="s">
-        <v>115</v>
-      </c>
-      <c r="D35" s="18" t="s">
-        <v>41</v>
-      </c>
-      <c r="E35" s="19"/>
-      <c r="F35" s="19"/>
-      <c r="G35" s="19"/>
-      <c r="H35" s="19" t="s">
-        <v>0</v>
-      </c>
-      <c r="I35" s="20"/>
-      <c r="J35"/>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A36" s="26" t="s">
-        <v>68</v>
-      </c>
-      <c r="B36" s="26" t="s">
-        <v>114</v>
-      </c>
-      <c r="C36" s="27" t="s">
-        <v>113</v>
-      </c>
-      <c r="D36" s="18" t="s">
+      <c r="C37" s="25" t="s">
+        <v>108</v>
+      </c>
+      <c r="D37" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="E36" s="19"/>
-      <c r="F36" s="19"/>
-      <c r="G36" s="19"/>
-      <c r="H36" s="19" t="s">
-        <v>0</v>
-      </c>
-      <c r="I36" s="20"/>
-      <c r="J36"/>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A37" s="28" t="s">
+      <c r="E37" s="17"/>
+      <c r="F37" s="17"/>
+      <c r="G37" s="17"/>
+      <c r="H37" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="I37" s="18"/>
+      <c r="J37"/>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A38" s="26" t="s">
         <v>80</v>
       </c>
-      <c r="B37" s="28"/>
-      <c r="C37" s="29"/>
-      <c r="D37" s="23" t="s">
+      <c r="B38" s="26"/>
+      <c r="C38" s="27"/>
+      <c r="D38" s="21" t="s">
         <v>43</v>
       </c>
-      <c r="E37" s="19"/>
-      <c r="F37" s="19"/>
-      <c r="G37" s="19"/>
-      <c r="H37" s="19" t="s">
-        <v>0</v>
-      </c>
-      <c r="I37" s="20"/>
-      <c r="J37"/>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B38" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="C38" s="1" t="s">
-        <v>128</v>
+      <c r="E38" s="17"/>
+      <c r="F38" s="17"/>
+      <c r="G38" s="17"/>
+      <c r="H38" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="I38" s="18"/>
+      <c r="J38"/>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B39" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="D39" s="28"/>
+      <c r="E39" s="1"/>
+      <c r="F39" s="1"/>
+      <c r="G39" s="1"/>
+      <c r="H39" s="1"/>
+      <c r="I39" s="4" t="s">
+        <v>141</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated descriptions and schism ids for some stations
</commit_message>
<xml_diff>
--- a/data/Stations_Importance.xlsx
+++ b/data/Stations_Importance.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\delta_salinity\scripts\DSP_code\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D42BBCAA-B560-4514-A2B1-9F9C2ADCF50A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1A2B7D7-33F3-4D22-8947-851DF4F131D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17790" xr2:uid="{DB7A9B06-FD48-4539-AA38-6D28440ECAB7}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25800" windowHeight="21150" xr2:uid="{DB7A9B06-FD48-4539-AA38-6D28440ECAB7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="158">
   <si>
     <t>Y</t>
   </si>
@@ -486,6 +486,30 @@
   </si>
   <si>
     <t>Threemile Slough near Rio Vista</t>
+  </si>
+  <si>
+    <t>bks</t>
+  </si>
+  <si>
+    <t>Barker Slough Pumping Plant</t>
+  </si>
+  <si>
+    <t>ges</t>
+  </si>
+  <si>
+    <t>Gsacramento R below Georgiana Slough</t>
+  </si>
+  <si>
+    <t>nmr</t>
+  </si>
+  <si>
+    <t>N Mokeulmne R near Walnut Grove</t>
+  </si>
+  <si>
+    <t>mru</t>
+  </si>
+  <si>
+    <t>Middle River at Undine Road</t>
   </si>
 </sst>
 </file>
@@ -588,7 +612,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -663,8 +687,6 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -702,17 +724,17 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{9F1BA903-751C-4660-B3EA-7CFC748037BB}" name="Table1" displayName="Table1" ref="D1:I39" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{9CA28F63-D4C8-4427-B844-EFFB884BEF7E}" name="Table13" displayName="Table13" ref="D1:I39" totalsRowShown="0">
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="D2:I38">
     <sortCondition ref="E1:E38"/>
   </sortState>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{02F85A5B-494A-43D0-A963-65DB30957B18}" name="DSM2 Description" dataDxfId="5"/>
-    <tableColumn id="2" xr3:uid="{4C7B2D15-6B0D-435B-BB38-D38566CCE77C}" name="SHOULD HAVE FOR CALSIM" dataDxfId="4"/>
-    <tableColumn id="4" xr3:uid="{3986071E-1297-4FE7-9CAE-654E061DDEF2}" name="STRUCTURAL" dataDxfId="3"/>
-    <tableColumn id="5" xr3:uid="{032429B3-7981-42C7-A43E-BD5E70692FDB}" name="??" dataDxfId="2"/>
-    <tableColumn id="3" xr3:uid="{3FD418F8-3AEA-4B06-8D87-70A6F07D7EBF}" name="EXCLUDE" dataDxfId="1"/>
-    <tableColumn id="6" xr3:uid="{5EE2F89F-E9EA-4CFE-84C4-F6B35C503B31}" name="Notes" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{6EDAB40C-B0CD-4759-A4D1-5EF652F689FD}" name="DSM2 Description" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{983AEF54-7F13-4CF6-AF87-55634BEC9EA1}" name="SHOULD HAVE FOR CALSIM" dataDxfId="4"/>
+    <tableColumn id="4" xr3:uid="{ACFBCF94-B4AE-460C-B118-733203D1E95B}" name="STRUCTURAL" dataDxfId="3"/>
+    <tableColumn id="5" xr3:uid="{32AFCDCF-D617-4570-A725-4E0D714D7037}" name="??" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{1164460F-B76F-456B-BF69-3AE8F76A8287}" name="EXCLUDE" dataDxfId="1"/>
+    <tableColumn id="6" xr3:uid="{F0C84339-D4DA-4C6C-802B-A00F9E4BBC07}" name="Notes" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1018,7 +1040,7 @@
   <dimension ref="A1:J39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I26" sqref="A26:I39"/>
+      <selection activeCell="D42" sqref="D42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1315,7 +1337,7 @@
       <c r="C13" s="13" t="s">
         <v>149</v>
       </c>
-      <c r="D13" s="29"/>
+      <c r="D13" s="7"/>
       <c r="E13" s="1" t="s">
         <v>0</v>
       </c>
@@ -1635,8 +1657,12 @@
       <c r="A28" s="22" t="s">
         <v>77</v>
       </c>
-      <c r="B28" s="22"/>
-      <c r="C28" s="23"/>
+      <c r="B28" s="22" t="s">
+        <v>150</v>
+      </c>
+      <c r="C28" s="23" t="s">
+        <v>151</v>
+      </c>
       <c r="D28" s="21" t="s">
         <v>33</v>
       </c>
@@ -1697,8 +1723,12 @@
       <c r="A31" s="19" t="s">
         <v>79</v>
       </c>
-      <c r="B31" s="19"/>
-      <c r="C31" s="20"/>
+      <c r="B31" s="19" t="s">
+        <v>152</v>
+      </c>
+      <c r="C31" s="20" t="s">
+        <v>153</v>
+      </c>
       <c r="D31" s="21" t="s">
         <v>36</v>
       </c>
@@ -1715,8 +1745,12 @@
       <c r="A32" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="B32" s="22"/>
-      <c r="C32" s="23"/>
+      <c r="B32" s="22" t="s">
+        <v>154</v>
+      </c>
+      <c r="C32" s="23" t="s">
+        <v>155</v>
+      </c>
       <c r="D32" s="21" t="s">
         <v>37</v>
       </c>
@@ -1843,8 +1877,12 @@
       <c r="A38" s="26" t="s">
         <v>80</v>
       </c>
-      <c r="B38" s="26"/>
-      <c r="C38" s="27"/>
+      <c r="B38" s="26" t="s">
+        <v>156</v>
+      </c>
+      <c r="C38" s="27" t="s">
+        <v>157</v>
+      </c>
       <c r="D38" s="21" t="s">
         <v>43</v>
       </c>
@@ -1864,7 +1902,6 @@
       <c r="C39" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="D39" s="28"/>
       <c r="E39" s="1"/>
       <c r="F39" s="1"/>
       <c r="G39" s="1"/>

</xml_diff>